<commit_message>
14/01 - adicionar melhor goleiro
</commit_message>
<xml_diff>
--- a/pelada_sabado_2025_01.xlsx
+++ b/pelada_sabado_2025_01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernando.almeida\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ritzferramentasltda-my.sharepoint.com/personal/fernando_almeida_ritzbrasil_com/Documents/Desktop/Nova pasta (2)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4F8BC1-6226-4183-A566-CBF7D1198137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FF4164-CC9B-4219-88F1-B402B001A279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
   <si>
     <t>Boneco</t>
   </si>
@@ -159,6 +159,27 @@
   </si>
   <si>
     <t>Raniery</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Leandrão</t>
+  </si>
+  <si>
+    <t>Geovane</t>
+  </si>
+  <si>
+    <t>Leah</t>
+  </si>
+  <si>
+    <t>Milton</t>
+  </si>
+  <si>
+    <t>Lucian</t>
+  </si>
+  <si>
+    <t>Melhor Goleiro</t>
   </si>
 </sst>
 </file>
@@ -485,11 +506,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -497,7 +518,7 @@
     <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -531,8 +552,11 @@
       <c r="K1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -563,8 +587,11 @@
       <c r="K2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -595,8 +622,11 @@
       <c r="K3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -627,8 +657,11 @@
       <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -659,8 +692,11 @@
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -691,8 +727,11 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -723,8 +762,11 @@
       <c r="K7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -755,8 +797,11 @@
       <c r="K8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -787,8 +832,11 @@
       <c r="K9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -819,8 +867,11 @@
       <c r="K10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -851,8 +902,11 @@
       <c r="K11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -883,8 +937,11 @@
       <c r="K12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -915,8 +972,11 @@
       <c r="K13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -947,8 +1007,11 @@
       <c r="K14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -979,8 +1042,11 @@
       <c r="K15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1009,6 +1075,9 @@
         <v>0</v>
       </c>
       <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
         <v>0</v>
       </c>
     </row>
@@ -1043,6 +1112,9 @@
       <c r="K17">
         <v>0</v>
       </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -1075,6 +1147,9 @@
       <c r="K18">
         <v>0</v>
       </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -1107,6 +1182,9 @@
       <c r="K19">
         <v>0</v>
       </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
@@ -1139,6 +1217,9 @@
       <c r="K20">
         <v>0</v>
       </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -1171,6 +1252,9 @@
       <c r="K21">
         <v>0</v>
       </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
@@ -1203,6 +1287,9 @@
       <c r="K22">
         <v>0</v>
       </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -1235,6 +1322,9 @@
       <c r="K23">
         <v>0</v>
       </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -1267,6 +1357,9 @@
       <c r="K24">
         <v>0</v>
       </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -1299,6 +1392,9 @@
       <c r="K25">
         <v>0</v>
       </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
       <c r="O25" s="1"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
@@ -1332,6 +1428,9 @@
       <c r="K26">
         <v>0</v>
       </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
       <c r="O26" s="1"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
@@ -1365,6 +1464,9 @@
       <c r="K27">
         <v>0</v>
       </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
       <c r="O27" s="1"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
@@ -1398,6 +1500,9 @@
       <c r="K28">
         <v>0</v>
       </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
       <c r="O28" s="1"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
@@ -1431,6 +1536,9 @@
       <c r="K29">
         <v>0</v>
       </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
       <c r="O29" s="1"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
@@ -1464,6 +1572,9 @@
       <c r="K30">
         <v>0</v>
       </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
       <c r="O30" s="1"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
@@ -1497,6 +1608,9 @@
       <c r="K31">
         <v>0</v>
       </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
       <c r="O31" s="1"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
@@ -1530,6 +1644,9 @@
       <c r="K32">
         <v>0</v>
       </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
       <c r="O32" s="1"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.35">
@@ -1563,6 +1680,9 @@
       <c r="K33">
         <v>0</v>
       </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
       <c r="O33" s="1"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.35">
@@ -1594,6 +1714,9 @@
         <v>0</v>
       </c>
       <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
         <v>0</v>
       </c>
       <c r="O34" s="1"/>
@@ -1629,6 +1752,9 @@
       <c r="K35">
         <v>0</v>
       </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
       <c r="O35" s="1"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.35">
@@ -1662,6 +1788,9 @@
       <c r="K36">
         <v>0</v>
       </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
       <c r="O36" s="1"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.35">
@@ -1693,6 +1822,9 @@
         <v>0</v>
       </c>
       <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
         <v>0</v>
       </c>
       <c r="O37" s="1"/>
@@ -1728,6 +1860,9 @@
       <c r="K38">
         <v>0</v>
       </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
       <c r="O38" s="1"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.35">
@@ -1761,6 +1896,9 @@
       <c r="K39">
         <v>0</v>
       </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
       <c r="O39" s="1"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.35">
@@ -1794,6 +1932,9 @@
       <c r="K40">
         <v>0</v>
       </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
       <c r="O40" s="1"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.35">
@@ -1827,6 +1968,9 @@
       <c r="K41">
         <v>0</v>
       </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
       <c r="O41" s="1"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.35">
@@ -1860,6 +2004,9 @@
       <c r="K42">
         <v>19</v>
       </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
       <c r="O42" s="1"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.35">
@@ -1893,13 +2040,783 @@
       <c r="K43">
         <v>17</v>
       </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
       <c r="O43" s="1"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
       <c r="O44" s="1"/>
     </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>4</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49">
+        <v>4</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>3</v>
+      </c>
+      <c r="E51">
+        <v>4</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>3</v>
+      </c>
+      <c r="E52">
+        <v>4</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53">
+        <v>4</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>3</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55">
+        <v>2</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>42</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56">
+        <v>3</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>34</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59">
+        <v>6</v>
+      </c>
+      <c r="D59">
+        <v>3</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>6</v>
+      </c>
+      <c r="D60">
+        <v>3</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>2</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61">
+        <v>6</v>
+      </c>
+      <c r="D61">
+        <v>3</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>3</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>36</v>
+      </c>
+      <c r="C62">
+        <v>6</v>
+      </c>
+      <c r="D62">
+        <v>3</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>3</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63">
+        <v>6</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64">
+        <v>6</v>
+      </c>
+      <c r="D64">
+        <v>5</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="F64">
+        <v>3</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>12</v>
+      </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>45</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65">
+        <v>5</v>
+      </c>
+      <c r="E65">
+        <v>6</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>18</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K446" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>